<commit_message>
docs : "Dialogue 수정"
</commit_message>
<xml_diff>
--- a/SecondHeeHeeMotGa/Assets/Resources/ExcelDB/DialogueDB.xlsx
+++ b/SecondHeeHeeMotGa/Assets/Resources/ExcelDB/DialogueDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramae\OneDrive\바탕 화면\기말고사\1학년\2학기\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramae\taemgit\Git20230925\hihisecondproject\SecondHeeHeeMotGa\Assets\Resources\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{206FE1E2-5CC2-43B3-A283-DE204E593312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C65E2D1-D85B-46F3-A9F0-B8C5225D7882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9432" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{652A8C2A-7F9B-4019-94BA-83C3A0987B3E}"/>
+    <workbookView minimized="1" xWindow="-144" yWindow="324" windowWidth="14712" windowHeight="11472" xr2:uid="{652A8C2A-7F9B-4019-94BA-83C3A0987B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="68">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,10 +83,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>휴학 신청은 했니~'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"하.. 알겠다고요.."</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,19 +115,195 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[알람 소리]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[띠링]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"헉!!"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"지각이다!!!!"</t>
+    <t>'딸~ 자퇴신청은 했니~'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(응? 내가 언제 잠들었었지?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(게임 내용이 재미가 없었나보다ㅎㅎ)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(근데 무슨 소리가 들리는 거같은데..)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(설마 침입자??!)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(슬쩍.. 눈 떠볼까..?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"일어났니?"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"뭐야!! 넌 누구야!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밍밍디 요정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room1Gray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>침입?자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"나?"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"난 밍밍디 요정이야"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"반응이 왜그래!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"난 널 도울 요정이라고!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"너가 뭘 돕겠다는 거야"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"너의 인생"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"???"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room2Gray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"앞으로 살아가면서"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"수많은 선택을 하며 살게 될거야"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"지금도 선택의 기로에 놓여있지 않아?"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"내가 도와줄게"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"이게 무슨소리야.."</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"방금 처음 본 널 뭘 믿고…"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"우리 처음 아니야!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"기억 못하는 구나?"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"어?"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"이건 중요치 않고!!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"바로 설명해줄게!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"어어어???"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"여긴 또 어디야!!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"..? 그래서 뭐하는 사람?"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"아니.. 사람이 아닌가..?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"네가 앞으로 어떻게 하면 되는지"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"시간이 별로 없어!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"한번만 설명 할 거니까 잘 들어"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"넌 앞으로 수 많은 사람을 만날거야"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"사람을 만날 때마다 또 수많은 '퍼즐'을 풀게 되겠지"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"난 네가 그'퍼즐'을 두려워하지 않았으면 좋겠어"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"그 '퍼즐'을 풀어 갈 수록 특별한 경험을 하게 될거야"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"나와의 '퍼즐'을 먼저 풀어볼까?"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"ㅁ..뭔소리야"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -511,16 +683,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9063FF04-4D74-4434-BBE5-1403F5DDD3F9}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="63.8984375" customWidth="1"/>
     <col min="5" max="5" width="13.69921875" customWidth="1"/>
     <col min="6" max="6" width="16.19921875" customWidth="1"/>
@@ -571,10 +743,12 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -591,10 +765,12 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -611,10 +787,12 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -631,10 +809,12 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -651,10 +831,12 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -671,10 +853,12 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -691,10 +875,12 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -711,10 +897,12 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -731,10 +919,12 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -751,14 +941,18 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
@@ -768,15 +962,17 @@
         <v>0</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
@@ -787,14 +983,18 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
@@ -805,14 +1005,18 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
@@ -822,13 +1026,19 @@
         <v>0</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
@@ -838,13 +1048,19 @@
         <v>0</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
@@ -854,27 +1070,41 @@
         <v>0</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="2">
+        <v>101</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
@@ -882,41 +1112,67 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="2">
+        <v>101</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2">
+        <v>101</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
@@ -924,13 +1180,19 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
@@ -938,13 +1200,515 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="2">
+        <v>102</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="2">
+        <v>102</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="2">
+        <v>102</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="2">
+        <v>101</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="2">
+        <v>103</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="2">
+        <v>103</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="2">
+        <v>103</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="2">
+        <v>103</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="2">
+        <v>101</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="2">
+        <v>101</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="2">
+        <v>104</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="2">
+        <v>104</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="2">
+        <v>104</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="2">
+        <v>101</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="2">
+        <v>103</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="2">
+        <v>103</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="2">
+        <v>103</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="2">
+        <v>103</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="2">
+        <v>103</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="2">
+        <v>103</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A51" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Feat: "Merge 시스템 구현"
</commit_message>
<xml_diff>
--- a/SecondHeeHeeMotGa/Assets/Resources/ExcelDB/DialogueDB.xlsx
+++ b/SecondHeeHeeMotGa/Assets/Resources/ExcelDB/DialogueDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anwlr\OneDrive\바탕 화면\Unity\hihiproject\HeeHeeMotGa\Assets\Resources\ExcelDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anwlr\OneDrive\바탕 화면\hihisecondproject\SecondHeeHeeMotGa\Assets\Resources\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D43A1A-561D-4D6A-8A5E-7A3E7746B4D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828FC885-3C30-4D3F-89F2-21057B9D4411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="74">
   <si>
     <t>tweenType</t>
   </si>
@@ -300,6 +300,10 @@
   </si>
   <si>
     <t>BackGround/Gray</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merge_Test</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -355,7 +359,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -370,9 +374,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,8 +653,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1403,7 +1404,7 @@
       <c r="B25" s="1">
         <v>0</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -2201,7 +2202,7 @@
         <v>-100</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>